<commit_message>
Seed chosen from sequence instead of fixed
</commit_message>
<xml_diff>
--- a/6-Changes.xlsx
+++ b/6-Changes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EF9B70-23EB-406F-9E58-8D2FC24E4790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3027919D-3B8E-4B62-819A-7D8401B2C33C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1212" yWindow="576" windowWidth="21828" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>no decay</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>0.1, 0.9</t>
+  </si>
+  <si>
+    <t>---&gt;</t>
+  </si>
+  <si>
+    <t>batch</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -203,12 +209,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,6 +402,18 @@
     <tableColumn id="6" xr3:uid="{301F987C-6C65-417A-8299-6EE565F164C8}" name="lr"/>
     <tableColumn id="7" xr3:uid="{16B833C5-144E-4C65-82A6-A9FD938EE435}" name="loss"/>
     <tableColumn id="8" xr3:uid="{EBFAF451-37F2-40E3-B3DB-8EB96EF2989C}" name="epochs"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CA3E5259-476E-495D-AD87-1C95A039B295}" name="Table3" displayName="Table3" ref="Q4:S5" totalsRowShown="0">
+  <autoFilter ref="Q4:S5" xr:uid="{6A7AA47F-E93F-47E7-AF9F-F419F746EAB2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{981B6DA0-B42D-439A-B2F9-526DD9960551}" name="batch"/>
+    <tableColumn id="2" xr3:uid="{5A6B337F-8399-4FF7-A7C6-5E75A3228881}" name="loss"/>
+    <tableColumn id="3" xr3:uid="{7EFEAA6F-10DD-4D71-94C5-B4E7DCB9A3EC}" name="epochs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -650,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,9 +698,10 @@
     <col min="10" max="10" width="10.21875" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" customWidth="1"/>
     <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -681,21 +714,21 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -729,14 +762,14 @@
       <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -773,8 +806,15 @@
       <c r="O3">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -808,8 +848,17 @@
       <c r="O4">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -846,9 +895,20 @@
       <c r="O5">
         <v>340</v>
       </c>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5">
+        <v>1152</v>
+      </c>
+      <c r="R5">
+        <v>0.210293099284172</v>
+      </c>
+      <c r="S5">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -883,7 +943,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -918,7 +978,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -953,7 +1013,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -991,7 +1051,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1029,7 +1089,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1124,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>23</v>
       </c>
@@ -1093,7 +1153,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>23</v>
       </c>
@@ -1122,7 +1182,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G14" t="s">
         <v>23</v>
       </c>
@@ -1151,7 +1211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>23</v>
       </c>
@@ -1180,7 +1240,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
         <v>23</v>
       </c>
@@ -1326,9 +1386,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="G1:M1"/>
+    <mergeCell ref="R3:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C13">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
@@ -1364,9 +1425,10 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>